<commit_message>
prepare bio and chemistry
</commit_message>
<xml_diff>
--- a/api/python/TaiGerTranscriptAnalyzerJS/database/Biology/BIO_Programs.xlsx
+++ b/api/python/TaiGerTranscriptAnalyzerJS/database/Biology/BIO_Programs.xlsx
@@ -8,15 +8,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miO8AT4kTlgHwf3/+ugnEYjVYujNw=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="jzJdBoEpkjco2MUhGodZu5L+JCJmreTbT2YAZDNcsbI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Program</t>
   </si>
@@ -24,25 +24,10 @@
     <t>Choose</t>
   </si>
   <si>
-    <t>Mannheim Data Science</t>
+    <t>TUM_CHEMICAL_BIOTECHNOLOGY</t>
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Mannheim Business Informatics</t>
-  </si>
-  <si>
-    <t>TUM Business Informatics</t>
-  </si>
-  <si>
-    <t>Tuebingen Machine Learning</t>
-  </si>
-  <si>
-    <t>TU_Berlin_Info_Sys_Mgmt</t>
-  </si>
-  <si>
-    <t>Uni Muenster Information System</t>
   </si>
 </sst>
 </file>
@@ -59,7 +44,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -313,53 +297,18 @@
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="3" ht="14.25" customHeight="1"/>
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
     <row r="8" ht="14.25" customHeight="1"/>
     <row r="9" ht="14.25" customHeight="1"/>
     <row r="10" ht="14.25" customHeight="1"/>
@@ -1348,14 +1297,9 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B1:B7">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B1:B2">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>